<commit_message>
Revert "Revert "Update 10月学習計画書_李子晗.xlsx""
This reverts commit 2d872473bb82c512769c7d6bcac592f7159ced04.
</commit_message>
<xml_diff>
--- a/進捗/10月学習計画書_李子晗.xlsx
+++ b/進捗/10月学習計画書_李子晗.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Li Zihan\Documents\GitHub\October_study\進捗\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED730314-910C-4F2F-9D8F-3D1B05855410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="学習計画書" sheetId="1" r:id="rId1"/>
     <sheet name="学習資料" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -350,7 +356,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -361,7 +367,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -372,7 +378,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -383,7 +389,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -394,7 +400,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -405,7 +411,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -416,7 +422,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -427,7 +433,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -464,7 +470,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -475,7 +481,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -486,7 +492,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -497,7 +503,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -508,7 +514,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -519,7 +525,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -530,7 +536,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -541,7 +547,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -578,7 +584,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -589,7 +595,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -600,7 +606,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -611,7 +617,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -622,7 +628,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -633,7 +639,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -644,7 +650,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -655,7 +661,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -692,7 +698,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -703,7 +709,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -714,7 +720,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -725,7 +731,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -736,7 +742,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -747,7 +753,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -758,7 +764,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -769,7 +775,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -806,7 +812,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -817,7 +823,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -828,7 +834,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -839,7 +845,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -850,7 +856,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -861,7 +867,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -872,7 +878,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -883,7 +889,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -920,7 +926,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -931,7 +937,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -942,7 +948,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -953,7 +959,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -964,7 +970,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -975,7 +981,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -986,7 +992,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -997,7 +1003,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1058,7 +1064,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
@@ -1066,14 +1072,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="游ゴシック"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1082,7 +1088,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="等线"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1097,7 +1103,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="等线"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1106,7 +1112,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="游ゴシック"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1128,7 +1134,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1555,28 +1561,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="19.8"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.36328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="60.375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.4">
+    <row r="1" spans="1:8" ht="20.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1588,7 +1594,7 @@
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
     </row>
-    <row r="2" spans="1:8" ht="26.4">
+    <row r="2" spans="1:8" ht="20.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1653,7 +1659,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="19.5">
       <c r="A5" s="4">
         <v>44110</v>
       </c>
@@ -1827,7 +1833,9 @@
       <c r="F11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="16">
+        <v>0.9</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1">
@@ -2274,14 +2282,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="19.8"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -2360,12 +2368,12 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A5" r:id="rId2"/>
-    <hyperlink ref="A11" r:id="rId3"/>
-    <hyperlink ref="A8" r:id="rId4"/>
-    <hyperlink ref="A13" r:id="rId5" display="https://www.youtube.com/playlist?list=PL9nxfq1tlKKlcx425yrc-17LiY0lcQBeC"/>
-    <hyperlink ref="A14" r:id="rId6"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A11" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="A8" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="A13" r:id="rId5" display="https://www.youtube.com/playlist?list=PL9nxfq1tlKKlcx425yrc-17LiY0lcQBeC" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="A14" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Update 10月学習計画書_李子晗.xlsx"""
This reverts commit 3c8e9258ab0654eff3bee0eddd9f8f315af923fa.
</commit_message>
<xml_diff>
--- a/進捗/10月学習計画書_李子晗.xlsx
+++ b/進捗/10月学習計画書_李子晗.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Li Zihan\Documents\GitHub\October_study\進捗\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED730314-910C-4F2F-9D8F-3D1B05855410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="学習計画書" sheetId="1" r:id="rId1"/>
     <sheet name="学習資料" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -356,9 +350,123 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>础</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 入</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>门</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>实战</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>教程 33-39</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
+      </rPr>
+      <t>練習</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Nodejs MongoDb Express 零基</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>础</t>
@@ -367,7 +475,121 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 入</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>门</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>实战</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>教程 6-10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>練習</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Nodejs MongoDb Express 零基</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>础</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -378,9 +600,123 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>门</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>实战</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>教程 11-15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
+      </rPr>
+      <t>練習</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Nodejs MongoDb Express 零基</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>础</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 入</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>门</t>
@@ -389,7 +725,121 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>实战</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>教程 16-18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>練習</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Nodejs MongoDb Express 零基</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>础</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 入</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>门</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -400,9 +850,123 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>实战</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>视频</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>教程 19-23</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
+      </rPr>
+      <t>練習</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Nodejs MongoDb Express 零基</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>础</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 入</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>门</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>实战</t>
@@ -411,7 +975,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -422,7 +986,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="游ゴシック"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -433,577 +997,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>教程 33-39</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>・</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>練習</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Nodejs MongoDb Express 零基</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>础</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 入</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>门</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>实战</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>教程 6-10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>・</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>練習</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Nodejs MongoDb Express 零基</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>础</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 入</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>门</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>实战</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>教程 11-15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>・</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>練習</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Nodejs MongoDb Express 零基</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>础</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 入</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>门</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>实战</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>教程 16-18</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>・</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>練習</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Nodejs MongoDb Express 零基</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>础</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 入</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>门</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>实战</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>教程 19-23</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>・</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>練習</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>Nodejs MongoDb Express 零基</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>础</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 入</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>门</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>实战</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>视频</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="游ゴシック"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1064,7 +1058,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
@@ -1072,14 +1066,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1088,7 +1082,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="游ゴシック"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1103,7 +1097,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="游ゴシック"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1112,7 +1106,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1134,7 +1128,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1561,28 +1555,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="19.8"/>
   <cols>
-    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="60.36328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25">
+    <row r="1" spans="1:8" ht="26.4">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1594,7 +1588,7 @@
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
     </row>
-    <row r="2" spans="1:8" ht="20.25">
+    <row r="2" spans="1:8" ht="26.4">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1659,7 +1653,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="19.5">
+    <row r="5" spans="1:8">
       <c r="A5" s="4">
         <v>44110</v>
       </c>
@@ -1833,9 +1827,7 @@
       <c r="F11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="16">
-        <v>0.9</v>
-      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1">
@@ -2282,14 +2274,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="19.8"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -2368,12 +2360,12 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A11" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="A8" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="A13" r:id="rId5" display="https://www.youtube.com/playlist?list=PL9nxfq1tlKKlcx425yrc-17LiY0lcQBeC" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="A14" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A5" r:id="rId2"/>
+    <hyperlink ref="A11" r:id="rId3"/>
+    <hyperlink ref="A8" r:id="rId4"/>
+    <hyperlink ref="A13" r:id="rId5" display="https://www.youtube.com/playlist?list=PL9nxfq1tlKKlcx425yrc-17LiY0lcQBeC"/>
+    <hyperlink ref="A14" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>